<commit_message>
Avance creacion de tablas para RDC01
</commit_message>
<xml_diff>
--- a/Analisis/procedimientos/procedimientos.xlsx
+++ b/Analisis/procedimientos/procedimientos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/procedimientos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A08B091C-4616-482D-8978-EE76077D56B7}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22ADF66D-31E7-4E16-B569-1F27AEA9E8E2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,15 +36,9 @@
     <t>Descripcion</t>
   </si>
   <si>
-    <t>val_interfaz_A01</t>
-  </si>
-  <si>
     <t>Procedimiento para validar calidad de informacion de la interfaz cartera_operaciones</t>
   </si>
   <si>
-    <t>val_interfaz_B01</t>
-  </si>
-  <si>
     <t>Procedimiento para validar calidad de informacion de la interfaz cuadro_operaciones</t>
   </si>
   <si>
@@ -52,6 +46,12 @@
   </si>
   <si>
     <t>Procedimiento para borrar datos de tablas usadas en los procesos diarios</t>
+  </si>
+  <si>
+    <t>val_interfaz_a01</t>
+  </si>
+  <si>
+    <t>val_interfaz_b01</t>
   </si>
 </sst>
 </file>
@@ -104,6 +104,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,10 +401,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -408,10 +412,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -419,10 +423,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Termino procedimiento RDC01 e RDC01 historico
</commit_message>
<xml_diff>
--- a/Analisis/procedimientos/procedimientos.xlsx
+++ b/Analisis/procedimientos/procedimientos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/procedimientos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A17BD56E-AA2B-4A3A-8ECF-FE7F3CA95676}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C079EC3-6998-44CF-8455-983B5D3B862D}"/>
   <bookViews>
-    <workbookView xWindow="-15210" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="procedimientos" sheetId="1" r:id="rId1"/>
+    <sheet name="Objetos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>schema</t>
   </si>
@@ -58,14 +59,82 @@
   </si>
   <si>
     <t>Procedimiento para la generacion del RDC01</t>
+  </si>
+  <si>
+    <t>Procedimiento</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>Tablas_involucradas</t>
+  </si>
+  <si>
+    <t>reporte</t>
+  </si>
+  <si>
+    <t>rdc01_texto</t>
+  </si>
+  <si>
+    <t>rdc01_detalle</t>
+  </si>
+  <si>
+    <t>rdc01_final</t>
+  </si>
+  <si>
+    <t>interface</t>
+  </si>
+  <si>
+    <t>cartera_operaciones</t>
+  </si>
+  <si>
+    <t>interno</t>
+  </si>
+  <si>
+    <t>tipo_persona_rel</t>
+  </si>
+  <si>
+    <t>operacion_titulo_rel</t>
+  </si>
+  <si>
+    <t>tabla_banco_126_rel</t>
+  </si>
+  <si>
+    <t>tipo_cambio</t>
+  </si>
+  <si>
+    <t>cuadro_operaciones</t>
+  </si>
+  <si>
+    <t>cartera_garantias</t>
+  </si>
+  <si>
+    <t>log_eventos</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>parametros_generales</t>
+  </si>
+  <si>
+    <t>rdc01_hist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,8 +162,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,4 +519,177 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2995A567-7CFD-4B3D-85CC-8FBB121F91D4}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Reapply "Issue #36""
This reverts commit b593879306406ceeca5ebc6063f166e6c9f109f0.
</commit_message>
<xml_diff>
--- a/Analisis/procedimientos/procedimientos.xlsx
+++ b/Analisis/procedimientos/procedimientos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/procedimientos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{456618F0-ED43-42F4-9E1C-55BCE7B22854}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9228CAB1-2C0A-4FF9-B405-4294C9E25094}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>schema</t>
   </si>
@@ -131,12 +131,6 @@
   </si>
   <si>
     <t>Procedimiento para validar calidad de informacion de la interfaz cartera_garantias</t>
-  </si>
-  <si>
-    <t>proceso.genera_hist_log</t>
-  </si>
-  <si>
-    <t>Procedimiento para generar historico de los log</t>
   </si>
 </sst>
 </file>
@@ -467,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,17 +548,6 @@
       </c>
       <c r="C7" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avance 2 Issue #52
Avance en calculo de exclusion por morosidad, cambios en RDC01, etc..
</commit_message>
<xml_diff>
--- a/Analisis/procedimientos/procedimientos.xlsx
+++ b/Analisis/procedimientos/procedimientos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/procedimientos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{456618F0-ED43-42F4-9E1C-55BCE7B22854}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76B35323-CA0A-4A54-9CB0-6FCCB26F6B70}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>schema</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>Procedimiento para generar historico de los log</t>
+  </si>
+  <si>
+    <t>excluir_por_morosidad</t>
+  </si>
+  <si>
+    <t>Procedimiento para calcular si las operaciones morosas tienen 5 años o mas</t>
   </si>
 </sst>
 </file>
@@ -467,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,6 +571,17 @@
       </c>
       <c r="C8" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>